<commit_message>
Add draft logo. Add mockups. Add about_us.md
</commit_message>
<xml_diff>
--- a/user_stories.xlsx
+++ b/user_stories.xlsx
@@ -5,20 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="271" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="431" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Specs" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Stories" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="objects_and_attr" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Questions" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="132">
   <si>
     <t>Scenario</t>
   </si>
@@ -128,6 +129,9 @@
     <t>signin</t>
   </si>
   <si>
+    <t>I can see my profile</t>
+  </si>
+  <si>
     <t>change password</t>
   </si>
   <si>
@@ -393,6 +397,24 @@
   </si>
   <si>
     <t>resume</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>Setup User Controller</t>
+  </si>
+  <si>
+    <t>some description of notes</t>
+  </si>
+  <si>
+    <t>2. check file</t>
+  </si>
+  <si>
+    <t>1.run CLI </t>
+  </si>
+  <si>
+    <t>rails generate controller users</t>
   </si>
 </sst>
 </file>
@@ -493,17 +515,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -525,18 +559,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="C2:C7 C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7142857142857"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9336734693878"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1938775510204"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.0663265306122"/>
@@ -590,8 +624,8 @@
   </sheetPr>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -600,664 +634,666 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1173469387755"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.5663265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.3316326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.2755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="44.3316326530612"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+    <row r="2" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="n">
+      <c r="F2" s="5"/>
+      <c r="G2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+    <row r="3" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+    <row r="4" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+    <row r="5" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="n">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="n">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+    <row r="8" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="n">
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="n">
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="n">
+      <c r="D10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="E11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
+      <c r="F21" s="5"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
+      <c r="D22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="D23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="D25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2" t="s">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+      <c r="E30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="C31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="E31" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="F31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="n">
+      <c r="A34" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="n">
+      <c r="A35" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="n">
+      <c r="A36" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="n">
+      <c r="A37" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1278,8 +1314,8 @@
   </sheetPr>
   <dimension ref="B1:E55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="1" sqref="C2:C7 B27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1294,13 +1330,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1308,7 +1344,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,7 +1352,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,464 +1360,464 @@
         <v>34</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="E16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="3" t="s">
         <v>95</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>78</v>
+        <v>95</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>78</v>
+        <v>99</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>78</v>
+        <v>99</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>108</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E54" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1803,8 +1839,8 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="C2:C7 B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1816,34 +1852,138 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.4489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>